<commit_message>
Finalization of the project
Improved In-Code Documentation
Improved Code Quality
Improved Code Readability
Improved Code Structure
Final Documentation added
Final Presentation added
</commit_message>
<xml_diff>
--- a/files/raw/Zeitplanung.xlsx
+++ b/files/raw/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fokko\source\repos\ict-335-praxisarbeit\files\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE6EB43-9BAF-4C74-A9CC-D1D22D3EC369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1228545F-0B84-4E09-9457-79282FF3C19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{1EA5CFC8-9728-41E1-8E28-D9D8C07954D4}"/>
   </bookViews>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E24D91-B141-486E-BF23-34263C9B75C6}">
   <dimension ref="A2:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,11 +1012,11 @@
       </c>
       <c r="D14" s="8">
         <f>SUM(D15:D19)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E14" s="9">
         <f>SUM(E15:E19) / COUNT(E15:E19)</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="10"/>
       <c r="N14" s="10"/>
@@ -1061,10 +1061,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="12"/>
     </row>
@@ -1076,10 +1076,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="12"/>
     </row>
@@ -1091,10 +1091,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="12"/>
     </row>
@@ -1106,10 +1106,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="12"/>
     </row>
@@ -1124,11 +1124,11 @@
       </c>
       <c r="D20" s="8">
         <f>SUM(D21:D21)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="9">
         <f>SUM(E21:E21) / COUNT(E21:E21)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1161,10 +1161,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="12"/>
     </row>
@@ -1179,11 +1179,11 @@
       </c>
       <c r="D22" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E22" s="9">
         <f>SUM(E23:E25) / COUNT(E23:E25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1215,10 +1215,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="12"/>
     </row>
@@ -1230,10 +1230,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="12"/>
     </row>
@@ -1245,10 +1245,10 @@
         <v>0.5</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="12"/>
     </row>
@@ -1262,11 +1262,11 @@
       </c>
       <c r="D26" s="15">
         <f>SUM(D6,D8,D12,D14,D20,D22)</f>
-        <v>11.5</v>
+        <v>23.5</v>
       </c>
       <c r="E26" s="16">
         <f>SUM(E6,E8,E12,E14,E20,E22) / COUNT(E6,E8,E12,E14,E20,E22)</f>
-        <v>0.53333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G26" s="17">
         <v>17</v>

</xml_diff>